<commit_message>
Update Civil Works Expenditurture
</commit_message>
<xml_diff>
--- a/Civilworks cost/LD/LD Annexes2.xlsx
+++ b/Civilworks cost/LD/LD Annexes2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Annex-II" sheetId="1" r:id="rId1"/>
@@ -2103,8 +2103,8 @@
   </sheetPr>
   <dimension ref="A1:D358"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6028,7 +6028,7 @@
   </sheetPr>
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>

</xml_diff>